<commit_message>
change the snowpack to skiresort
</commit_message>
<xml_diff>
--- a/hxb-interface.xlsx
+++ b/hxb-interface.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="389">
   <si>
     <t>URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -383,9 +383,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>snowpacks</t>
-  </si>
-  <si>
     <t>雪场列表</t>
     <rPh sb="0" eb="1">
       <t>xue'chang</t>
@@ -413,13 +410,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>位置</t>
-    <rPh sb="0" eb="1">
-      <t>wei'zhi</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>人员状况</t>
     <rPh sb="0" eb="1">
       <t>ren'yuan</t>
@@ -443,15 +433,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>——snowpackId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>——hasBus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>——location</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -486,10 +468,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/snowpack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>页数</t>
     <rPh sb="0" eb="1">
       <t>ye'shu</t>
@@ -549,18 +527,6 @@
   </si>
   <si>
     <t>根据当前用户的位置信息，获取其位置所在城市的周边雪场列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/snowpack/near</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/snowpack/all</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/snowpack/often</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -668,18 +634,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>snowpackId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snowpackTrailPic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>——snowpackName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>雪场雪道图</t>
     <rPh sb="0" eb="1">
       <t>xue'chang</t>
@@ -691,10 +645,6 @@
   </si>
   <si>
     <t>activitys</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snowpackName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1264,10 +1214,6 @@
   </si>
   <si>
     <t>spToken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snowpackId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1533,10 +1479,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/snowpack/simple</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>获取雪场简要信息</t>
     <rPh sb="0" eb="1">
       <t>huo'qu</t>
@@ -1553,10 +1495,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>snowpackName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>雪场名称</t>
     <rPh sb="0" eb="1">
       <t>xue'chang</t>
@@ -1590,10 +1528,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>snowpackSimples</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>雪场简讯列表</t>
     <rPh sb="0" eb="1">
       <t>xue'chang</t>
@@ -1607,19 +1541,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>——snowpackId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>——snowpackName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>——location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>——snowpackTeachFee</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1637,10 +1559,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>snowpackId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>滑雪场ID</t>
     <rPh sb="0" eb="1">
       <t>hua'xue</t>
@@ -1756,10 +1674,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/snowpack/activity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/activity/newTeach</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1968,10 +1882,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>snowpackName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>滑雪场名称</t>
     <rPh sb="0" eb="1">
       <t>hua'xue'c</t>
@@ -2326,14 +2236,6 @@
     <rPh sb="2" eb="3">
       <t>nei'rong</t>
     </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/snowpack/bus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/snowpack/myBus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2391,14 +2293,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/snowpack/busSite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/snowpack/busDetail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>activityBusId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2452,15 +2346,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/snowpack/busJoin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>POST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/snowpack/busQuit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2577,10 +2463,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>名称</t>
     <rPh sb="0" eb="1">
       <t>ming'cheng</t>
@@ -2635,6 +2517,106 @@
   </si>
   <si>
     <t>userId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>——address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地址</t>
+    <rPh sb="0" eb="1">
+      <t>di'zhi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>——skiresortId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>——skiresortName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skiresortName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trailPic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skiresortName</t>
+  </si>
+  <si>
+    <t>skiresortName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>trailPic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/skiresort/activity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/skiresort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/skiresort/all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/skiresort/often</t>
+  </si>
+  <si>
+    <t>skiresorts</t>
+  </si>
+  <si>
+    <t>skiresortId</t>
+  </si>
+  <si>
+    <t>/skiresort/bus</t>
+  </si>
+  <si>
+    <t>/skiresort/busSite</t>
+  </si>
+  <si>
+    <t>/skiresort/busJoin</t>
+  </si>
+  <si>
+    <t>/skiresort/myBus</t>
+  </si>
+  <si>
+    <t>/skiresort/busDetail</t>
+  </si>
+  <si>
+    <t>/skiresort/busQuit</t>
+  </si>
+  <si>
+    <t>/skiresort/simple</t>
+  </si>
+  <si>
+    <t>skiresortSimples</t>
+  </si>
+  <si>
+    <t>——skiresortId</t>
+  </si>
+  <si>
+    <t>——skiresortName</t>
+  </si>
+  <si>
+    <t>——skiresortTeachFee</t>
+  </si>
+  <si>
+    <t>/skiresort/near</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2751,7 +2733,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2768,6 +2750,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="25">
@@ -3076,7 +3061,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3090,7 +3075,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3109,7 +3094,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>373</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -3117,7 +3102,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3133,10 +3118,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>388</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -3144,7 +3129,7 @@
     </row>
     <row r="8" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -3152,7 +3137,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3168,10 +3153,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>374</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
@@ -3179,7 +3164,7 @@
     </row>
     <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3215,7 +3200,7 @@
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>57</v>
@@ -3301,10 +3286,10 @@
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>375</v>
+      </c>
+      <c r="B28" t="s">
         <v>58</v>
-      </c>
-      <c r="B28" t="s">
-        <v>59</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s">
@@ -3313,10 +3298,10 @@
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>364</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s">
@@ -3325,77 +3310,77 @@
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>365</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s">
         <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s">
         <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>361</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>362</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="49" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s">
         <v>43</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3440,10 +3425,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3470,10 +3455,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -3485,46 +3470,46 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
       <c r="B9" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
       <c r="B10" t="s">
-        <v>364</v>
+        <v>336</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
       <c r="B11" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>367</v>
+        <v>339</v>
       </c>
       <c r="B12" t="s">
-        <v>368</v>
+        <v>340</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -3622,13 +3607,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>340</v>
+        <v>380</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3655,10 +3640,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -3673,7 +3658,7 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>57</v>
@@ -3744,10 +3729,10 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="B15" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
@@ -3756,10 +3741,10 @@
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
@@ -3768,85 +3753,85 @@
     </row>
     <row r="17" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
         <v>43</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s">
         <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s">
@@ -3856,10 +3841,10 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
@@ -3869,17 +3854,17 @@
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s">
         <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3919,13 +3904,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>348</v>
+        <v>381</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3952,10 +3937,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -3967,10 +3952,10 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -4036,51 +4021,51 @@
     </row>
     <row r="15" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="B16" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="B17" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="E17" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="B19" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -4120,10 +4105,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="B3" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4150,10 +4135,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -4165,10 +4150,10 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -4269,10 +4254,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4302,7 +4287,7 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -4373,18 +4358,18 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>383</v>
+        <v>354</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
@@ -4393,85 +4378,85 @@
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
@@ -4481,10 +4466,10 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s">
@@ -4494,17 +4479,17 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
         <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4544,10 +4529,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4577,7 +4562,7 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -4588,7 +4573,7 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -4651,36 +4636,36 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
       <c r="B14" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
       <c r="B15" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
@@ -4689,85 +4674,85 @@
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s">
         <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
@@ -4777,10 +4762,10 @@
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s">
@@ -4790,17 +4775,17 @@
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s">
         <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4840,10 +4825,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4873,7 +4858,7 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -4884,7 +4869,7 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -4947,36 +4932,36 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="B14" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
       <c r="B15" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>375</v>
+        <v>347</v>
       </c>
       <c r="B16" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
@@ -4985,85 +4970,85 @@
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s">
         <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
@@ -5073,10 +5058,10 @@
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s">
@@ -5086,17 +5071,17 @@
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s">
         <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -5137,13 +5122,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>383</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5175,7 +5160,7 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -5258,19 +5243,19 @@
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>221</v>
+        <v>384</v>
       </c>
       <c r="B17" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>223</v>
+        <v>385</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
@@ -5278,10 +5263,10 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>386</v>
       </c>
       <c r="B19" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>11</v>
@@ -5289,23 +5274,23 @@
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="B20" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>226</v>
+        <v>387</v>
       </c>
       <c r="B21" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="C21" s="2"/>
       <c r="E21" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -5356,10 +5341,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
@@ -5389,10 +5374,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -5403,79 +5388,79 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>376</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B11" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="B12" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B15" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B16" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -5602,10 +5587,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -5632,10 +5617,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -5721,192 +5706,192 @@
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>229</v>
+        <v>376</v>
       </c>
       <c r="B19" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>217</v>
+        <v>368</v>
       </c>
       <c r="B20" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B22" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="B23" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B24" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="B25" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B26" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B27" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B28" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B29" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="B30" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="B31" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="C31" s="2"/>
       <c r="E31" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="B32" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="B33" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="B34" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B35" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B37" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="B38" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="C38" s="2"/>
     </row>
@@ -5926,7 +5911,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5956,13 +5941,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C3" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -5989,53 +5974,53 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>366</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>362</v>
       </c>
       <c r="C9" s="2"/>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>379</v>
+        <v>351</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2"/>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>367</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2"/>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -6152,7 +6137,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -6182,10 +6167,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
         <v>252</v>
-      </c>
-      <c r="B7" t="s">
-        <v>273</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
@@ -6196,7 +6181,7 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -6208,7 +6193,7 @@
         <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -6333,10 +6318,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -6363,10 +6348,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
         <v>252</v>
-      </c>
-      <c r="B7" t="s">
-        <v>273</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
@@ -6377,7 +6362,7 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -6389,7 +6374,7 @@
         <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -6463,81 +6448,81 @@
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>278</v>
+        <v>368</v>
       </c>
       <c r="B17" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="B19" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="B20" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B21" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B22" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B23" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="B24" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="B25" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -6578,10 +6563,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -6608,10 +6593,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
         <v>252</v>
-      </c>
-      <c r="B7" t="s">
-        <v>273</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
@@ -6622,19 +6607,19 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
@@ -6643,19 +6628,19 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C10" s="2"/>
       <c r="E10" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -6769,10 +6754,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -6799,10 +6784,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
         <v>252</v>
-      </c>
-      <c r="B7" t="s">
-        <v>273</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
@@ -6813,19 +6798,19 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
@@ -6834,19 +6819,19 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C10" s="2"/>
       <c r="E10" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -6958,10 +6943,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>386</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -6988,10 +6973,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -7002,10 +6987,10 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>387</v>
+        <v>358</v>
       </c>
       <c r="B8" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -7083,117 +7068,117 @@
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>217</v>
+        <v>368</v>
       </c>
       <c r="B19" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B21" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B22" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B23" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B24" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>385</v>
+        <v>356</v>
       </c>
       <c r="B25" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B27" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B28" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B29" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="B30" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -7238,10 +7223,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -7268,10 +7253,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
         <v>252</v>
-      </c>
-      <c r="B7" t="s">
-        <v>273</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
@@ -7282,19 +7267,19 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
@@ -7303,19 +7288,19 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C10" s="2"/>
       <c r="E10" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -7427,10 +7412,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -7457,10 +7442,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -7531,18 +7516,18 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
       <c r="B14" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>299</v>
+        <v>277</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
@@ -7551,85 +7536,85 @@
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
@@ -7639,10 +7624,10 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s">
@@ -7652,17 +7637,17 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
         <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -7702,7 +7687,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
@@ -7732,10 +7717,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -7746,10 +7731,10 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
@@ -7760,10 +7745,10 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
       <c r="B9" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>39</v>
@@ -7772,15 +7757,15 @@
         <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
       <c r="B10" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>40</v>
@@ -7789,12 +7774,12 @@
         <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>310</v>
+        <v>288</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -7908,10 +7893,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>311</v>
+        <v>289</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -7938,10 +7923,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>290</v>
       </c>
       <c r="B7" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -8012,18 +7997,18 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
       <c r="B14" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>299</v>
+        <v>277</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
@@ -8032,85 +8017,85 @@
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
         <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
@@ -8120,10 +8105,10 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s">
@@ -8133,17 +8118,17 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
         <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -8183,10 +8168,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -8213,10 +8198,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -8287,18 +8272,18 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="B14" t="s">
-        <v>313</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>316</v>
+        <v>294</v>
       </c>
       <c r="B15" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
@@ -8309,19 +8294,19 @@
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="B16" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="B17" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>39</v>
@@ -8330,15 +8315,15 @@
         <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>40</v>
@@ -8347,12 +8332,12 @@
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
@@ -8393,8 +8378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8424,10 +8409,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>371</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -8435,7 +8420,7 @@
     </row>
     <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -8462,10 +8447,10 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>376</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>57</v>
@@ -8479,7 +8464,7 @@
         <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>57</v>
@@ -8562,28 +8547,28 @@
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>369</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>370</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
@@ -8592,10 +8577,10 @@
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s">
@@ -8604,86 +8589,86 @@
     </row>
     <row r="23" spans="1:6" ht="49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s">
         <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s">
@@ -8693,10 +8678,10 @@
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s">
@@ -8706,17 +8691,17 @@
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s">
         <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -8762,7 +8747,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -8795,7 +8780,7 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>389</v>
+        <v>360</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -8807,7 +8792,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -8884,28 +8869,28 @@
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>326</v>
+        <v>304</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>11</v>
@@ -8917,10 +8902,10 @@
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>32</v>
@@ -8931,10 +8916,10 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>11</v>
@@ -8945,24 +8930,24 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>327</v>
+        <v>305</v>
       </c>
       <c r="B23" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
       <c r="B24" t="s">
-        <v>329</v>
+        <v>307</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s">
@@ -8972,17 +8957,17 @@
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="B25" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s">
         <v>43</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>333</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -9031,10 +9016,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="B3" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -9064,7 +9049,7 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -9076,24 +9061,24 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="B8" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -9215,19 +9200,19 @@
     </row>
     <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -9254,7 +9239,7 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -9266,7 +9251,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -9343,10 +9328,10 @@
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -9354,10 +9339,10 @@
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
@@ -9365,24 +9350,24 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s">
@@ -9392,10 +9377,10 @@
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B21" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
@@ -9440,21 +9425,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -9467,33 +9452,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -9522,33 +9507,33 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
@@ -9562,21 +9547,21 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
@@ -9601,7 +9586,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9622,21 +9607,21 @@
         <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -9646,33 +9631,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -9718,33 +9703,33 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>
@@ -9758,15 +9743,15 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -9822,7 +9807,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -9866,7 +9851,7 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
@@ -9900,10 +9885,10 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>11</v>
@@ -9915,10 +9900,10 @@
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>32</v>
@@ -9929,10 +9914,10 @@
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
@@ -10009,7 +9994,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10034,13 +10019,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>339</v>
+        <v>377</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -10067,10 +10052,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>179</v>
+        <v>376</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -10145,51 +10130,51 @@
     </row>
     <row r="15" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="B17" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="E17" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="B19" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -10229,13 +10214,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>347</v>
+        <v>378</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -10262,10 +10247,10 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>179</v>
+        <v>376</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -10340,38 +10325,38 @@
     </row>
     <row r="15" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B18" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>